<commit_message>
mass balance file and update all locations
</commit_message>
<xml_diff>
--- a/alllocations.xlsx
+++ b/alllocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weert\Documents\GitHub\MAIO_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8C8AAC-ACB8-4B19-9AE5-B3DE7B01B19D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE9B0B7-946A-4ADA-A5C0-B5D70FF6BC01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="15">
   <si>
     <t>S4</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>in sigma units</t>
+  </si>
+  <si>
+    <t>Values from file</t>
+  </si>
+  <si>
+    <t>Annual velocities</t>
   </si>
 </sst>
 </file>
@@ -907,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI38"/>
+  <dimension ref="A1:AJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +934,7 @@
     <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3.8462000000000003E-2</v>
       </c>
@@ -955,7 +961,7 @@
         <v>92.735246532886947</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2.9</v>
       </c>
@@ -982,7 +988,7 @@
         <v>90.165822187424979</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1022,14 @@
       <c r="AH3" t="s">
         <v>12</v>
       </c>
+      <c r="AI3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1990.5</v>
       </c>
@@ -1121,8 +1133,11 @@
         <f>(B4*$A$1+$E$1*F4+$I$1*J4+$M$1*N4+$Q$1*R4+$U$1*V4+$Y$1*Z4)/SUM($A$1:$Y$1)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ4">
+        <v>96.19</v>
+      </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1991.5</v>
       </c>
@@ -1226,8 +1241,11 @@
         <f t="shared" ref="AI5:AI34" si="9">(B5*$A$1+$E$1*F5+$I$1*J5+$M$1*N5+$Q$1*R5+$U$1*V5+$Y$1*Z5)/SUM($A$1:$Y$1)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ5">
+        <v>93.48</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1992.5</v>
       </c>
@@ -1332,7 +1350,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1993.5</v>
       </c>
@@ -1436,8 +1454,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ7">
+        <v>96.43</v>
+      </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1994.5</v>
       </c>
@@ -1542,7 +1563,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1995.5</v>
       </c>
@@ -1646,8 +1667,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ9">
+        <v>95.36</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1996.5</v>
       </c>
@@ -1751,8 +1775,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ10">
+        <v>99.9</v>
+      </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1997.5</v>
       </c>
@@ -1856,8 +1883,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ11">
+        <v>92.45</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1998.5</v>
       </c>
@@ -1961,8 +1991,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ12">
+        <v>90.43</v>
+      </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1999.5</v>
       </c>
@@ -2066,8 +2099,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ13">
+        <v>90.56</v>
+      </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2000.5</v>
       </c>
@@ -2171,8 +2207,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ14">
+        <v>83.86</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2001.5</v>
       </c>
@@ -2276,8 +2315,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ15">
+        <v>91.3</v>
+      </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2002.5</v>
       </c>
@@ -2381,8 +2423,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ16">
+        <v>90.23</v>
+      </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2003.5</v>
       </c>
@@ -2486,8 +2531,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ17">
+        <v>90.19</v>
+      </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2004.5</v>
       </c>
@@ -2591,8 +2639,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ18">
+        <v>88.26</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2005.5</v>
       </c>
@@ -2696,8 +2747,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ19">
+        <v>90.16</v>
+      </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2006.5</v>
       </c>
@@ -2805,8 +2859,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ20">
+        <v>87.06</v>
+      </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2007.5</v>
       </c>
@@ -2914,8 +2971,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ21">
+        <v>85.47</v>
+      </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2008.5</v>
       </c>
@@ -3028,8 +3088,11 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
+      <c r="AJ22">
+        <v>90.86</v>
+      </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2009.5</v>
       </c>
@@ -3148,8 +3211,11 @@
         <f t="shared" si="9"/>
         <v>93.590110939823461</v>
       </c>
+      <c r="AJ23">
+        <v>90.5</v>
+      </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2010.5</v>
       </c>
@@ -3268,8 +3334,11 @@
         <f t="shared" si="9"/>
         <v>95.320202330647447</v>
       </c>
+      <c r="AJ24">
+        <v>86.69</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2011.5</v>
       </c>
@@ -3388,8 +3457,11 @@
         <f t="shared" si="9"/>
         <v>90.883352102901085</v>
       </c>
+      <c r="AJ25">
+        <v>89.55</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2012.5</v>
       </c>
@@ -3503,7 +3575,7 @@
         <v>94.763467045522006</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2013.5</v>
       </c>
@@ -3623,7 +3695,7 @@
         <v>88.099179779681265</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2014.5</v>
       </c>
@@ -3743,7 +3815,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2015.5</v>
       </c>
@@ -3861,7 +3933,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2016.5</v>
       </c>
@@ -3972,7 +4044,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2017.5</v>
       </c>
@@ -4091,7 +4163,7 @@
         <v>89.740510807266958</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2018.5</v>
       </c>
@@ -4263,6 +4335,7 @@
         <v>93.383520760539483</v>
       </c>
       <c r="AB34" s="1"/>
+      <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
       <c r="AI34">
         <f t="shared" si="9"/>

</xml_diff>